<commit_message>
Added graphs for talk 10/6/15
</commit_message>
<xml_diff>
--- a/MODEL/Human_Model_Data_Quickgraphs.xlsx
+++ b/MODEL/Human_Model_Data_Quickgraphs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="-33200" yWindow="-4880" windowWidth="20480" windowHeight="12320" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Human_Model_Data.csv" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="25">
   <si>
     <t>Source</t>
   </si>
@@ -83,12 +83,24 @@
   <si>
     <t>5 VERBS</t>
   </si>
+  <si>
+    <t>Prettier V5 down here</t>
+  </si>
+  <si>
+    <t>Include Subject</t>
+  </si>
+  <si>
+    <t>Include Object</t>
+  </si>
+  <si>
+    <t>Include Verb</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -112,6 +124,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -130,21 +149,38 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -168,7 +204,17 @@
   <c:chart>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.0464859148041277"/>
+          <c:y val="0.0787037037037037"/>
+          <c:w val="0.934880544823201"/>
+          <c:h val="0.737531350247886"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
@@ -370,11 +416,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2139161784"/>
-        <c:axId val="2124837976"/>
+        <c:axId val="2116770136"/>
+        <c:axId val="2119652392"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2139161784"/>
+        <c:axId val="2116770136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -383,7 +429,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2124837976"/>
+        <c:crossAx val="2119652392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -391,7 +437,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2124837976"/>
+        <c:axId val="2119652392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -403,7 +449,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2139161784"/>
+        <c:crossAx val="2116770136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -694,11 +740,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2139437624"/>
-        <c:axId val="2139998456"/>
+        <c:axId val="2121707480"/>
+        <c:axId val="2121327848"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2139437624"/>
+        <c:axId val="2121707480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -707,7 +753,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2139998456"/>
+        <c:crossAx val="2121327848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -715,7 +761,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2139998456"/>
+        <c:axId val="2121327848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -727,7 +773,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2139437624"/>
+        <c:crossAx val="2121707480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -962,11 +1008,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2098777640"/>
-        <c:axId val="-2099358792"/>
+        <c:axId val="2063610744"/>
+        <c:axId val="2108884584"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2098777640"/>
+        <c:axId val="2063610744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -975,7 +1021,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2099358792"/>
+        <c:crossAx val="2108884584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -983,7 +1029,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2099358792"/>
+        <c:axId val="2108884584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -994,11 +1040,444 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2098777640"/>
+        <c:crossAx val="2063610744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="122"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="22"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Human_Model_Data.csv!$F$60</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1_6</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Human_Model_Data.csv!$G$59:$I$59</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Include Subject</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Include Object</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Include Verb</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Human_Model_Data.csv!$G$60:$I$60</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.22619</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.9026</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.87121</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Human_Model_Data.csv!$F$61</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2_5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Human_Model_Data.csv!$G$59:$I$59</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Include Subject</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Include Object</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Include Verb</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Human_Model_Data.csv!$G$61:$I$61</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.40476</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.79762</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.79762</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Human_Model_Data.csv!$F$62</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>3_4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Human_Model_Data.csv!$G$59:$I$59</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Include Subject</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Include Object</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Include Verb</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Human_Model_Data.csv!$G$62:$I$62</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.55357</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.68254</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.76389</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Human_Model_Data.csv!$F$63</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>4_3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Human_Model_Data.csv!$G$59:$I$59</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Include Subject</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Include Object</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Include Verb</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Human_Model_Data.csv!$G$63:$I$63</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.68254</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.55357</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.76389</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Human_Model_Data.csv!$F$64</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>5_2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4">
+                <a:lumMod val="40000"/>
+                <a:lumOff val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Human_Model_Data.csv!$G$59:$I$59</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Include Subject</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Include Object</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Include Verb</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Human_Model_Data.csv!$G$64:$I$64</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.79762</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.40476</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.79762</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Human_Model_Data.csv!$F$65</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>6_1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4">
+                <a:lumMod val="20000"/>
+                <a:lumOff val="80000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Human_Model_Data.csv!$G$59:$I$59</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Include Subject</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Include Object</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Include Verb</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Human_Model_Data.csv!$G$65:$I$65</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.9026</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.22619</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.87121</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="2122620472"/>
+        <c:axId val="2118495240"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2122620472"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2118495240"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2118495240"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2122620472"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -1098,6 +1577,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>812800</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1428,10 +1937,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K55"/>
+  <dimension ref="A1:K77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="N64" sqref="N64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2231,7 +2740,7 @@
         <v>0.28909000000000001</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:9">
       <c r="A49" t="s">
         <v>16</v>
       </c>
@@ -2245,7 +2754,7 @@
         <v>0.14491999999999999</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:9">
       <c r="A50" t="s">
         <v>16</v>
       </c>
@@ -2259,7 +2768,7 @@
         <v>0.99605999999999995</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:9">
       <c r="A51" t="s">
         <v>16</v>
       </c>
@@ -2273,7 +2782,7 @@
         <v>0.99343999999999999</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:9">
       <c r="A52" t="s">
         <v>16</v>
       </c>
@@ -2287,7 +2796,7 @@
         <v>0.99212999999999996</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:9">
       <c r="A53" t="s">
         <v>16</v>
       </c>
@@ -2301,7 +2810,7 @@
         <v>0.99212999999999996</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:9">
       <c r="A54" t="s">
         <v>16</v>
       </c>
@@ -2315,7 +2824,7 @@
         <v>0.99343999999999999</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:9">
       <c r="A55" t="s">
         <v>16</v>
       </c>
@@ -2327,6 +2836,292 @@
       </c>
       <c r="D55">
         <v>0.99605999999999995</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9">
+      <c r="B58" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9">
+      <c r="G59" t="s">
+        <v>22</v>
+      </c>
+      <c r="H59" t="s">
+        <v>23</v>
+      </c>
+      <c r="I59" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9">
+      <c r="B60" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D60" s="1">
+        <v>0.22619</v>
+      </c>
+      <c r="F60" t="s">
+        <v>8</v>
+      </c>
+      <c r="G60" s="1">
+        <v>0.22619</v>
+      </c>
+      <c r="H60" s="1">
+        <v>0.90259999999999996</v>
+      </c>
+      <c r="I60" s="1">
+        <v>0.87121000000000004</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9">
+      <c r="B61" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D61" s="1">
+        <v>0.40476000000000001</v>
+      </c>
+      <c r="F61" t="s">
+        <v>9</v>
+      </c>
+      <c r="G61" s="1">
+        <v>0.40476000000000001</v>
+      </c>
+      <c r="H61" s="1">
+        <v>0.79762</v>
+      </c>
+      <c r="I61" s="1">
+        <v>0.79762</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9">
+      <c r="B62" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D62" s="1">
+        <v>0.55357000000000001</v>
+      </c>
+      <c r="F62" t="s">
+        <v>10</v>
+      </c>
+      <c r="G62" s="1">
+        <v>0.55357000000000001</v>
+      </c>
+      <c r="H62" s="1">
+        <v>0.68254000000000004</v>
+      </c>
+      <c r="I62" s="1">
+        <v>0.76388999999999996</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9">
+      <c r="B63" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D63" s="1">
+        <v>0.68254000000000004</v>
+      </c>
+      <c r="F63" t="s">
+        <v>11</v>
+      </c>
+      <c r="G63" s="1">
+        <v>0.68254000000000004</v>
+      </c>
+      <c r="H63" s="1">
+        <v>0.55357000000000001</v>
+      </c>
+      <c r="I63" s="1">
+        <v>0.76388999999999996</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9">
+      <c r="B64" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D64" s="1">
+        <v>0.79762</v>
+      </c>
+      <c r="F64" t="s">
+        <v>12</v>
+      </c>
+      <c r="G64" s="1">
+        <v>0.79762</v>
+      </c>
+      <c r="H64" s="1">
+        <v>0.40476000000000001</v>
+      </c>
+      <c r="I64" s="1">
+        <v>0.79762</v>
+      </c>
+    </row>
+    <row r="65" spans="2:9">
+      <c r="B65" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D65" s="1">
+        <v>0.90259999999999996</v>
+      </c>
+      <c r="F65" t="s">
+        <v>13</v>
+      </c>
+      <c r="G65" s="1">
+        <v>0.90259999999999996</v>
+      </c>
+      <c r="H65" s="1">
+        <v>0.22619</v>
+      </c>
+      <c r="I65" s="1">
+        <v>0.87121000000000004</v>
+      </c>
+    </row>
+    <row r="66" spans="2:9">
+      <c r="B66" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D66" s="1">
+        <v>0.90259999999999996</v>
+      </c>
+    </row>
+    <row r="67" spans="2:9">
+      <c r="B67" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D67" s="1">
+        <v>0.79762</v>
+      </c>
+    </row>
+    <row r="68" spans="2:9">
+      <c r="B68" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D68" s="1">
+        <v>0.68254000000000004</v>
+      </c>
+    </row>
+    <row r="69" spans="2:9">
+      <c r="B69" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D69" s="1">
+        <v>0.55357000000000001</v>
+      </c>
+    </row>
+    <row r="70" spans="2:9">
+      <c r="B70" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D70" s="1">
+        <v>0.40476000000000001</v>
+      </c>
+    </row>
+    <row r="71" spans="2:9">
+      <c r="B71" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D71" s="1">
+        <v>0.22619</v>
+      </c>
+    </row>
+    <row r="72" spans="2:9">
+      <c r="B72" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D72" s="1">
+        <v>0.87121000000000004</v>
+      </c>
+    </row>
+    <row r="73" spans="2:9">
+      <c r="B73" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D73" s="1">
+        <v>0.79762</v>
+      </c>
+    </row>
+    <row r="74" spans="2:9">
+      <c r="B74" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D74" s="1">
+        <v>0.76388999999999996</v>
+      </c>
+    </row>
+    <row r="75" spans="2:9">
+      <c r="B75" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D75" s="1">
+        <v>0.76388999999999996</v>
+      </c>
+    </row>
+    <row r="76" spans="2:9">
+      <c r="B76" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D76" s="1">
+        <v>0.79762</v>
+      </c>
+    </row>
+    <row r="77" spans="2:9">
+      <c r="B77" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D77" s="1">
+        <v>0.87121000000000004</v>
       </c>
     </row>
   </sheetData>

</xml_diff>